<commit_message>
Update files about components.
</commit_message>
<xml_diff>
--- a/DATA/components/All_components.xlsx
+++ b/DATA/components/All_components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Models_In_Python\Work_Model v4.0\DATA\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444308CC-E2D3-45D5-82F1-E0F0EDA9D6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8BE991-EDEB-42E5-BC75-BB5F0C05C1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Водород-радикал</t>
   </si>
@@ -87,12 +87,6 @@
     <t>Вода</t>
   </si>
   <si>
-    <t>rad</t>
-  </si>
-  <si>
-    <t>mol</t>
-  </si>
-  <si>
     <t>H*</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>Мольная доля</t>
   </si>
   <si>
-    <t>Тип</t>
-  </si>
-  <si>
     <t>Формула</t>
   </si>
   <si>
@@ -184,6 +175,9 @@
   </si>
   <si>
     <t>Массовая доля</t>
+  </si>
+  <si>
+    <t>Молекула</t>
   </si>
 </sst>
 </file>
@@ -272,7 +266,7 @@
     <tableColumn id="2" xr3:uid="{24F3D4F1-7A15-4B6C-B390-A9CDD2A29503}" name="Молярная масса" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{C9426D55-F589-423D-83E1-D7BDA3B45D09}" name="Мольная доля" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{C84B6E1F-0111-40B7-A5F6-25721BAD373A}" name="Массовая доля" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{D6D2E2D5-D613-4121-B260-65E9996F3ABB}" name="Тип" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D6D2E2D5-D613-4121-B260-65E9996F3ABB}" name="Молекула" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{B0216310-4BCB-4AEE-A169-EA9F1F06BABE}" name="Формула" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -563,22 +557,22 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -594,11 +588,12 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
@@ -617,11 +612,12 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
@@ -640,11 +636,12 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
+      <c r="E4" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
@@ -663,11 +660,12 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
+      <c r="E5" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
@@ -686,11 +684,12 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
+      <c r="E6" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -706,11 +705,12 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
+      <c r="E7" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -726,11 +726,12 @@
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
+      <c r="E8" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -746,11 +747,12 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
+      <c r="E9" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,11 +768,12 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>18</v>
+      <c r="E10" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -786,11 +789,12 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>18</v>
+      <c r="E11" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -806,11 +810,12 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>17</v>
+      <c r="E12" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -826,16 +831,17 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
+      <c r="E13" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3">
         <v>54.091800689697301</v>
@@ -846,16 +852,17 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>18</v>
+      <c r="E14" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3">
         <v>56.107700347900398</v>
@@ -866,16 +873,17 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>18</v>
+      <c r="E15" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3">
         <v>57.116</v>
@@ -886,11 +894,12 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>17</v>
+      <c r="E16" s="1" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -906,16 +915,17 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>18</v>
+      <c r="E17" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3">
         <v>58.124000549316399</v>
@@ -926,11 +936,12 @@
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
+      <c r="E18" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -946,11 +957,12 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>18</v>
+      <c r="E19" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -966,11 +978,12 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>18</v>
+      <c r="E20" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -986,11 +999,12 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>18</v>
+      <c r="E21" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1006,11 +1020,12 @@
       <c r="D22" s="1">
         <v>0</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>18</v>
+      <c r="E22" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rename column in xlsx-flie for create the class Reactions and Components.
</commit_message>
<xml_diff>
--- a/DATA/components/All_components.xlsx
+++ b/DATA/components/All_components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Models_In_Python\Work_Model v4.0\DATA\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8BE991-EDEB-42E5-BC75-BB5F0C05C1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6F97C7-ECDF-4E78-8D5C-96FA2C095B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Водород-радикал</t>
   </si>
@@ -135,18 +135,6 @@
     <t>H2O</t>
   </si>
   <si>
-    <t>Компонент</t>
-  </si>
-  <si>
-    <t>Молярная масса</t>
-  </si>
-  <si>
-    <t>Мольная доля</t>
-  </si>
-  <si>
-    <t>Формула</t>
-  </si>
-  <si>
     <t>C4H6-1,3</t>
   </si>
   <si>
@@ -174,10 +162,16 @@
     <t>i-C4H10</t>
   </si>
   <si>
-    <t>Массовая доля</t>
-  </si>
-  <si>
-    <t>Молекула</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>molar_mass</t>
+  </si>
+  <si>
+    <t>formula</t>
   </si>
 </sst>
 </file>
@@ -226,13 +220,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -256,18 +244,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F51CEFAD-1530-4E08-8CEF-240C4347C5EE}" name="Таблица1" displayName="Таблица1" ref="A1:F22" totalsRowShown="0">
-  <autoFilter ref="A1:F22" xr:uid="{F51CEFAD-1530-4E08-8CEF-240C4347C5EE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F51CEFAD-1530-4E08-8CEF-240C4347C5EE}" name="Таблица1" displayName="Таблица1" ref="A1:D22" totalsRowShown="0">
+  <autoFilter ref="A1:D22" xr:uid="{F51CEFAD-1530-4E08-8CEF-240C4347C5EE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
     <sortCondition ref="B1:B22"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F47786AE-67FB-4042-9F50-97FD3B99509E}" name="Компонент"/>
-    <tableColumn id="2" xr3:uid="{24F3D4F1-7A15-4B6C-B390-A9CDD2A29503}" name="Молярная масса" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C9426D55-F589-423D-83E1-D7BDA3B45D09}" name="Мольная доля" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{C84B6E1F-0111-40B7-A5F6-25721BAD373A}" name="Массовая доля" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{D6D2E2D5-D613-4121-B260-65E9996F3ABB}" name="Молекула" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{B0216310-4BCB-4AEE-A169-EA9F1F06BABE}" name="Формула" dataDxfId="0"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F47786AE-67FB-4042-9F50-97FD3B99509E}" name="name"/>
+    <tableColumn id="2" xr3:uid="{24F3D4F1-7A15-4B6C-B390-A9CDD2A29503}" name="molar_mass" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C9426D55-F589-423D-83E1-D7BDA3B45D09}" name="type" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C84B6E1F-0111-40B7-A5F6-25721BAD373A}" name="formula" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -539,7 +525,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,22 +543,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -582,19 +562,15 @@
       <c r="B2" s="3">
         <v>1.00800001621246</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="b">
+      <c r="C2" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
       <c r="I2" s="1"/>
@@ -606,19 +582,15 @@
       <c r="B3" s="3">
         <v>2.0160000324249299</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="C3" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
       <c r="I3" s="1"/>
@@ -630,19 +602,15 @@
       <c r="B4" s="3">
         <v>15.0349000692367</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="b">
+      <c r="C4" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="1"/>
@@ -654,19 +622,15 @@
       <c r="B5" s="3">
         <v>16.042900085449201</v>
       </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="C5" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
@@ -678,19 +642,15 @@
       <c r="B6" s="3">
         <v>18.015000000000001</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="C6" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -699,19 +659,15 @@
       <c r="B7" s="3">
         <v>26.038000106811499</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="C7" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -720,19 +676,15 @@
       <c r="B8" s="3">
         <v>28.0538005828857</v>
       </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="C8" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -741,19 +693,15 @@
       <c r="B9" s="3">
         <v>29.061900496482799</v>
       </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="b">
+      <c r="C9" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -762,19 +710,15 @@
       <c r="B10" s="3">
         <v>30.069900512695298</v>
       </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="C10" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -783,19 +727,15 @@
       <c r="B11" s="3">
         <v>42.080600738525398</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="C11" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -804,19 +744,15 @@
       <c r="B12" s="3">
         <v>43.089000105857799</v>
       </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="b">
+      <c r="C12" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -825,82 +761,66 @@
       <c r="B13" s="3">
         <v>44.097000122070298</v>
       </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="C13" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3">
         <v>54.091800689697301</v>
       </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="C14" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3">
         <v>56.107700347900398</v>
       </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="C15" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3">
         <v>57.116</v>
       </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1" t="b">
+      <c r="C16" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -909,40 +829,32 @@
       <c r="B17" s="3">
         <v>58.124000549316399</v>
       </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="C17" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B18" s="3">
         <v>58.124000549316399</v>
       </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="C18" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -951,19 +863,15 @@
       <c r="B19" s="3">
         <v>78.113400100000007</v>
       </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="C19" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -972,19 +880,15 @@
       <c r="B20" s="3">
         <v>92.140300100000005</v>
       </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="C20" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -993,19 +897,15 @@
       <c r="B21" s="3">
         <v>104.1512</v>
       </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="C21" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1014,19 +914,15 @@
       <c r="B22" s="3">
         <v>106.16719999999999</v>
       </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="C22" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Updating the reading and processing of components data.
</commit_message>
<xml_diff>
--- a/DATA/components/All_components.xlsx
+++ b/DATA/components/All_components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Models_In_Python\Work_Model v4.0\DATA\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6F97C7-ECDF-4E78-8D5C-96FA2C095B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDBC674-7D68-4206-AF0A-230EA40C20C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,9 +162,6 @@
     <t>i-C4H10</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>formula</t>
+  </si>
+  <si>
+    <t>molecular</t>
   </si>
 </sst>
 </file>
@@ -252,7 +252,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F47786AE-67FB-4042-9F50-97FD3B99509E}" name="name"/>
     <tableColumn id="2" xr3:uid="{24F3D4F1-7A15-4B6C-B390-A9CDD2A29503}" name="molar_mass" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C9426D55-F589-423D-83E1-D7BDA3B45D09}" name="type" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C9426D55-F589-423D-83E1-D7BDA3B45D09}" name="molecular" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{C84B6E1F-0111-40B7-A5F6-25721BAD373A}" name="formula" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,16 +543,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>